<commit_message>
First working version of HISTORIC PRECIPITATION, or the hp modifier from the command line.
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\dosan_daily_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F398E74A-095A-44FB-8319-1E20C9836914}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4166CFB-30BA-405E-A4A6-A2D25D8B73A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="1932" windowWidth="17280" windowHeight="8964" xr2:uid="{7F61EDE7-CB94-45C5-83B8-2106FB1B135E}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>The input and output folders for the simulated WTD raster must be the same. The script handles the issue of selecting the right file.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>WTD_input_and_output_folder</t>
   </si>
@@ -76,6 +73,18 @@
   </si>
   <si>
     <t>data/Strat4/DTM_metres_clip.tif</t>
+  </si>
+  <si>
+    <t>historic_precipitation</t>
+  </si>
+  <si>
+    <t>Optional. In order to run the model with historical data, execute the program in the command line as "python daily_map -hp". The model will run with all the historical data contined in the file specified in Path. In order to change the range of the simulation, carefully edit the .csv file to the range required. It is crucial to maintain the format. When doing so, the water table  begins the simulation at the surface, i.e., in fully saturated conditions.</t>
+  </si>
+  <si>
+    <t>data/Dayun_weather_1-11-19_12-00_AM_1_Year_1583925430_v2.csv</t>
+  </si>
+  <si>
+    <t>input</t>
   </si>
 </sst>
 </file>
@@ -427,71 +436,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F49BA472-FFBD-41DC-9472-8CD8ECD904A2}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Imam's canal raster in data/Strat4/new_canal_raster.tif
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\dosan_daily_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4166CFB-30BA-405E-A4A6-A2D25D8B73A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E06AC1-5777-4BA2-B186-BF9D29C42D99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="1932" windowWidth="17280" windowHeight="8964" xr2:uid="{7F61EDE7-CB94-45C5-83B8-2106FB1B135E}"/>
+    <workbookView xWindow="4980" yWindow="1440" windowWidth="17280" windowHeight="8964" xr2:uid="{7F61EDE7-CB94-45C5-83B8-2106FB1B135E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>parameters</t>
   </si>
   <si>
-    <t>data/Strat4/canals_clip.tif</t>
-  </si>
-  <si>
     <t>data/Strat4/Peattypedepth_clip.tif</t>
   </si>
   <si>
@@ -85,6 +82,9 @@
   </si>
   <si>
     <t>input</t>
+  </si>
+  <si>
+    <t>data/Strat4/new_canal_raster.tif</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -465,10 +465,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -476,10 +476,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -487,10 +487,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -498,10 +498,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -509,21 +509,21 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>